<commit_message>
updated the localization sheet by removing fields that are CRM related
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55059
</commit_message>
<xml_diff>
--- a/SOM/Documents/CRM Documetnation/BPM Data for Localization.xlsx
+++ b/SOM/Documents/CRM Documetnation/BPM Data for Localization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name=" Contact-Subscription Requests" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="Complaints" sheetId="8" r:id="rId6"/>
     <sheet name="Others" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="466">
   <si>
     <t>English</t>
   </si>
@@ -34,27 +34,9 @@
     <t>ST Notes</t>
   </si>
   <si>
-    <t>Contacts</t>
-  </si>
-  <si>
-    <t>List</t>
-  </si>
-  <si>
-    <t>Dashboards</t>
-  </si>
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>New Contact</t>
-  </si>
-  <si>
     <t>Individual</t>
   </si>
   <si>
-    <t>Customer Type</t>
-  </si>
-  <si>
     <t>Residential</t>
   </si>
   <si>
@@ -82,129 +64,21 @@
     <t>Please fill all required fields</t>
   </si>
   <si>
-    <t>Actions</t>
-  </si>
-  <si>
-    <t>Select multiple records</t>
-  </si>
-  <si>
-    <t>Show duplicate contacts</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>Add filter</t>
-  </si>
-  <si>
-    <t>Show folders</t>
-  </si>
-  <si>
-    <t>Switch to advanced mode</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>View</t>
-  </si>
-  <si>
-    <t>Set up summaries</t>
-  </si>
-  <si>
-    <t>Select fields to display</t>
-  </si>
-  <si>
-    <t>Open Dashboards</t>
-  </si>
-  <si>
-    <t>Open section wizard</t>
-  </si>
-  <si>
-    <t>Set up section cases</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Copy</t>
-  </si>
-  <si>
-    <t>Print</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
-    <t>Cancel</t>
-  </si>
-  <si>
-    <t>Contact name</t>
-  </si>
-  <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>Job title</t>
-  </si>
-  <si>
-    <t>Business phone</t>
-  </si>
-  <si>
-    <t>Mobile phone</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Customer Info</t>
-  </si>
-  <si>
     <t>Customer Personal Data</t>
   </si>
   <si>
     <t>Designation</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Birth Date</t>
-  </si>
-  <si>
-    <t>Birth Place</t>
-  </si>
-  <si>
-    <t>Middle Name</t>
-  </si>
-  <si>
     <t>Mother Name</t>
   </si>
   <si>
     <t>Career</t>
   </si>
   <si>
-    <t>Enter a value</t>
-  </si>
-  <si>
     <t>Document Info</t>
   </si>
   <si>
-    <t>Customer Billing Info</t>
-  </si>
-  <si>
-    <t>Customer ID</t>
-  </si>
-  <si>
     <t>Customer category</t>
   </si>
   <si>
@@ -217,21 +91,6 @@
     <t>Customer File Properties</t>
   </si>
   <si>
-    <t>Created On</t>
-  </si>
-  <si>
-    <t>Modified On</t>
-  </si>
-  <si>
-    <t>CRM ID</t>
-  </si>
-  <si>
-    <t>Created By</t>
-  </si>
-  <si>
-    <t>Modified By</t>
-  </si>
-  <si>
     <t>Customer Document ID</t>
   </si>
   <si>
@@ -247,75 +106,27 @@
     <t>Value entered doesn't match the field format</t>
   </si>
   <si>
-    <t>Customer Address</t>
-  </si>
-  <si>
-    <t>State Province</t>
-  </si>
-  <si>
     <t>District</t>
   </si>
   <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>Town</t>
   </si>
   <si>
-    <t>Building Number</t>
-  </si>
-  <si>
     <t>Floor Number</t>
   </si>
   <si>
-    <t>Billing Address ID</t>
-  </si>
-  <si>
-    <t>Customer Contact Info</t>
-  </si>
-  <si>
-    <t>Home Phone</t>
-  </si>
-  <si>
     <t>Fax Number</t>
   </si>
   <si>
     <t>User Settings</t>
   </si>
   <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>User CSO</t>
-  </si>
-  <si>
     <t>Switch Id</t>
   </si>
   <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>No data</t>
-  </si>
-  <si>
     <t>Field "{0}" : Enter a value</t>
   </si>
   <si>
-    <t>Feed</t>
-  </si>
-  <si>
-    <t>Publish</t>
-  </si>
-  <si>
-    <t>what are you working on?</t>
-  </si>
-  <si>
-    <t>This page contains unsaved changes. Do you still wish to leave the page?</t>
-  </si>
-  <si>
     <t>Billing Info</t>
   </si>
   <si>
@@ -328,18 +139,12 @@
     <t>Financial disputes</t>
   </si>
   <si>
-    <t>Installment invoice</t>
-  </si>
-  <si>
     <t>Collection Status</t>
   </si>
   <si>
     <t>Due Date</t>
   </si>
   <si>
-    <t>Details</t>
-  </si>
-  <si>
     <t>Bill Cycle</t>
   </si>
   <si>
@@ -364,15 +169,9 @@
     <t>Complaint</t>
   </si>
   <si>
-    <t>Starting Process</t>
-  </si>
-  <si>
     <t>Technical Step</t>
   </si>
   <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
@@ -439,15 +238,6 @@
     <t>Request History</t>
   </si>
   <si>
-    <t>Contract Requests</t>
-  </si>
-  <si>
-    <t>Line Subscription Request Details</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -484,9 +274,6 @@
     <t>Print Contract</t>
   </si>
   <si>
-    <t>Leased Line Request Details</t>
-  </si>
-  <si>
     <t>CSO is not commercial, you cannot create a leased line contract</t>
   </si>
   <si>
@@ -565,9 +352,6 @@
     <t>Print Configuration</t>
   </si>
   <si>
-    <t>Attachments and Notes</t>
-  </si>
-  <si>
     <t>Microwave Team</t>
   </si>
   <si>
@@ -712,18 +496,12 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Core services</t>
   </si>
   <si>
     <t>Check Consistency</t>
   </si>
   <si>
-    <t>check Availability</t>
-  </si>
-  <si>
     <t xml:space="preserve">Request Info </t>
   </si>
   <si>
@@ -742,36 +520,12 @@
     <t>Sequence Number</t>
   </si>
   <si>
-    <t>Drag File Here</t>
-  </si>
-  <si>
-    <t>Add Link</t>
-  </si>
-  <si>
-    <t>Add link on knowledge base</t>
-  </si>
-  <si>
-    <t>Delete Picture</t>
-  </si>
-  <si>
-    <t>Add picture</t>
-  </si>
-  <si>
     <t xml:space="preserve">Current Contact Time: 11:15 AM Damascus (GMT + 2:00) </t>
   </si>
   <si>
     <t>Segment</t>
   </si>
   <si>
-    <t>Set up access rights</t>
-  </si>
-  <si>
-    <t>Follow the feed</t>
-  </si>
-  <si>
-    <t>Unfollow the feed</t>
-  </si>
-  <si>
     <t>Update with social networks data</t>
   </si>
   <si>
@@ -805,9 +559,6 @@
     <t>First Number</t>
   </si>
   <si>
-    <t>You shoul pay : xxxx $</t>
-  </si>
-  <si>
     <t>No free DSLAM ports available and unable to add to waiting list (non syrian customer)</t>
   </si>
   <si>
@@ -817,18 +568,12 @@
     <t>Confirm</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Contract balance</t>
   </si>
   <si>
     <t xml:space="preserve">Free unit </t>
   </si>
   <si>
-    <t xml:space="preserve">Unbilled Amount </t>
-  </si>
-  <si>
     <t>Activation Date</t>
   </si>
   <si>
@@ -841,9 +586,6 @@
     <t>Status Date</t>
   </si>
   <si>
-    <t xml:space="preserve">CSO </t>
-  </si>
-  <si>
     <t>عسكري, اجنبي, سوري, سوري/فلسطيني</t>
   </si>
   <si>
@@ -871,9 +613,6 @@
     <t>if a field is requried and is not set on saving</t>
   </si>
   <si>
-    <t>This is BPM online field</t>
-  </si>
-  <si>
     <t>Media interface connector</t>
   </si>
   <si>
@@ -976,9 +715,6 @@
     <t>Line Termination</t>
   </si>
   <si>
-    <t>Reason</t>
-  </si>
-  <si>
     <t>Reason is mandatory</t>
   </si>
   <si>
@@ -1027,12 +763,6 @@
     <t>Friends and Family</t>
   </si>
   <si>
-    <t>Percentage field is required</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Create PABX </t>
-  </si>
-  <si>
     <t>Secondary contracts</t>
   </si>
   <si>
@@ -1213,9 +943,6 @@
     <t>Wireless extensions</t>
   </si>
   <si>
-    <t>wireless network</t>
-  </si>
-  <si>
     <t>Additional type</t>
   </si>
   <si>
@@ -1282,9 +1009,6 @@
     <t>Sub Region</t>
   </si>
   <si>
-    <t>User Name</t>
-  </si>
-  <si>
     <t>User Actions</t>
   </si>
   <si>
@@ -1561,15 +1285,6 @@
     <t>A boolean in Contact Take over to check whether both customers are available or not (Original and Target)</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Password Confirmation</t>
-  </si>
-  <si>
-    <t>Password doesn’t Match</t>
-  </si>
-  <si>
     <t>There is no difference between the services</t>
   </si>
   <si>
@@ -1621,12 +1336,6 @@
     <t>One or more services should be selected</t>
   </si>
   <si>
-    <t>Order By</t>
-  </si>
-  <si>
-    <t>List in Leased Line Termination</t>
-  </si>
-  <si>
     <t>Telephony Contracts</t>
   </si>
   <si>
@@ -1655,6 +1364,60 @@
   </si>
   <si>
     <t>Carrier contract is on multiplexer. The line should be moved to be able to continue.</t>
+  </si>
+  <si>
+    <t>New Customer</t>
+  </si>
+  <si>
+    <t>Segment Type</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Can be VIP or Residential</t>
+  </si>
+  <si>
+    <t>When creating a contact that is not an ST customer, may be a sponsor or a user in the system</t>
+  </si>
+  <si>
+    <t>Mr or Mrs.</t>
+  </si>
+  <si>
+    <t>Customer Id</t>
+  </si>
+  <si>
+    <t>Contact Info</t>
+  </si>
+  <si>
+    <t>CSO</t>
+  </si>
+  <si>
+    <t>The office that users work at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice Installment </t>
+  </si>
+  <si>
+    <t>Initiating a new request</t>
+  </si>
+  <si>
+    <t>used as comments on a task</t>
+  </si>
+  <si>
+    <t>Line Subscription</t>
+  </si>
+  <si>
+    <t>Leased Line</t>
+  </si>
+  <si>
+    <t>Check Availability</t>
+  </si>
+  <si>
+    <t>You should pay : xxxx $</t>
+  </si>
+  <si>
+    <t>Wireless network</t>
   </si>
 </sst>
 </file>
@@ -1690,9 +1453,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1840,8 +1606,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D278" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="A1:D278"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D201" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A1:D201"/>
   <tableColumns count="4">
     <tableColumn id="1" name="English" dataDxfId="39"/>
     <tableColumn id="2" name="Arabic" dataDxfId="38"/>
@@ -1866,8 +1632,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="A1:D19" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:D19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="A1:D17" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A1:D17"/>
   <tableColumns count="4">
     <tableColumn id="1" name="English" dataDxfId="27"/>
     <tableColumn id="2" name="Arabic" dataDxfId="26"/>
@@ -1879,8 +1645,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table357" displayName="Table357" ref="A1:D33" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:D33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table357" displayName="Table357" ref="A1:D31" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:D31"/>
   <tableColumns count="4">
     <tableColumn id="1" name="English" dataDxfId="21"/>
     <tableColumn id="2" name="Arabic" dataDxfId="20"/>
@@ -1918,13 +1684,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table32" displayName="Table32" ref="A1:D94" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D94"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table32" displayName="Table32" ref="A1:D90" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D90"/>
   <tableColumns count="4">
     <tableColumn id="1" name="English" dataDxfId="3"/>
     <tableColumn id="2" name="Arabic" dataDxfId="2"/>
-    <tableColumn id="3" name="Vanrise Notes" dataDxfId="0"/>
-    <tableColumn id="4" name="ST Notes" dataDxfId="1"/>
+    <tableColumn id="3" name="Vanrise Notes" dataDxfId="1"/>
+    <tableColumn id="4" name="ST Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2217,7 +1983,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D278"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2248,1456 +2014,1087 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
+      <c r="C3" s="1" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>449</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>274</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>455</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>37</v>
+      <c r="A35" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>456</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>458</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>277</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>279</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>280</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>281</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>79</v>
+        <v>461</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="92" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="93" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="C127" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
+      <c r="C154" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
+    <row r="162" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
+      <c r="C162" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
+      <c r="C163" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
+      <c r="C164" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
+      <c r="C169" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>186</v>
+        <v>331</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>189</v>
+        <v>176</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C191" s="1" t="s">
-        <v>284</v>
+        <v>178</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A226" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A227" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C227" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A229" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A263" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C263" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A265" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A266" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A267" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A268" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A271" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C272" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="1" t="s">
-        <v>273</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3735,117 +3132,117 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>294</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>295</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>296</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>297</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>298</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>299</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>300</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>301</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>302</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>303</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>304</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>305</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>306</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>307</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>308</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>314</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>309</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>310</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>311</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>312</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>315</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>313</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3858,11 +3255,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3889,92 +3286,82 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>316</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>317</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>318</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>319</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>320</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>321</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>322</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>323</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>324</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>325</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>326</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>327</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>328</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>330</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>332</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3987,11 +3374,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4018,177 +3405,167 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>333</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>334</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>335</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>336</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>337</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>338</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>339</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>340</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>341</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>342</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>343</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>344</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>346</v>
+        <v>258</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>362</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>349</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>350</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>351</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>352</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>353</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>354</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>355</v>
+        <v>273</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>356</v>
+        <v>274</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>363</v>
+        <v>275</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>368</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>366</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>365</v>
+        <v>268</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>367</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>357</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>369</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>361</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -4205,7 +3582,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4232,70 +3609,70 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>370</v>
+        <v>280</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>418</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>371</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>372</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>373</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>374</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>375</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>376</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>377</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>378</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>379</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>380</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>381</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>382</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -4312,7 +3689,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4339,177 +3716,177 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>383</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>384</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>385</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>386</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>387</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>388</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>389</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>390</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>391</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>392</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>393</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>394</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>395</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>396</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>397</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>398</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>399</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>400</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>401</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>402</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>403</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>404</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>405</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>406</v>
+        <v>315</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>407</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>408</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>409</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>410</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>411</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>412</v>
+        <v>321</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>413</v>
+        <v>322</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>414</v>
+        <v>323</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>415</v>
+        <v>324</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>416</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>417</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -4522,10 +3899,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4552,931 +3929,891 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>424</v>
+        <v>332</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>425</v>
+        <v>333</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>426</v>
+        <v>334</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>427</v>
+        <v>335</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>428</v>
+        <v>336</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>429</v>
+        <v>337</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>430</v>
+        <v>338</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>431</v>
+        <v>339</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>432</v>
+        <v>340</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>433</v>
+        <v>341</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>434</v>
+        <v>342</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>435</v>
+        <v>343</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>436</v>
+        <v>344</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>437</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>438</v>
+        <v>346</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>439</v>
+        <v>347</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>440</v>
+        <v>348</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>441</v>
+        <v>349</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>442</v>
+        <v>350</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>443</v>
+        <v>351</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>444</v>
+        <v>352</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>439</v>
+        <v>347</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>445</v>
+        <v>353</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>439</v>
+        <v>347</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>386</v>
+        <v>296</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>446</v>
+        <v>354</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>447</v>
+        <v>355</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>446</v>
+        <v>354</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>448</v>
+        <v>356</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>449</v>
+        <v>357</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>450</v>
+        <v>358</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>449</v>
+        <v>357</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>451</v>
+        <v>359</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>452</v>
+        <v>360</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>453</v>
+        <v>361</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>452</v>
+        <v>360</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>454</v>
+        <v>362</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>452</v>
+        <v>360</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>455</v>
+        <v>363</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>456</v>
+        <v>364</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>457</v>
+        <v>365</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>458</v>
+        <v>366</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>459</v>
+        <v>367</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>458</v>
+        <v>366</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>460</v>
+        <v>368</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>458</v>
+        <v>366</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>461</v>
+        <v>369</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>458</v>
+        <v>366</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>462</v>
+        <v>370</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>463</v>
+        <v>371</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>464</v>
+        <v>372</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>465</v>
+        <v>373</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>466</v>
+        <v>374</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>467</v>
+        <v>375</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>468</v>
+        <v>376</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>469</v>
+        <v>377</v>
       </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>470</v>
+        <v>378</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>471</v>
+        <v>379</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>472</v>
+        <v>380</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>473</v>
+        <v>381</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>474</v>
+        <v>382</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>475</v>
+        <v>383</v>
       </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>476</v>
+        <v>384</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>475</v>
+        <v>383</v>
       </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>477</v>
+        <v>385</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>478</v>
+        <v>386</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>479</v>
+        <v>387</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>478</v>
+        <v>386</v>
       </c>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>480</v>
+        <v>388</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>481</v>
+        <v>389</v>
       </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>482</v>
+        <v>390</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>483</v>
+        <v>391</v>
       </c>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>484</v>
+        <v>392</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>486</v>
+        <v>394</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>487</v>
+        <v>395</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>489</v>
+        <v>397</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>490</v>
+        <v>398</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>491</v>
+        <v>399</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>492</v>
+        <v>400</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>493</v>
+        <v>401</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>494</v>
+        <v>402</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>495</v>
+        <v>403</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>496</v>
+        <v>404</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>497</v>
+        <v>405</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>498</v>
+        <v>406</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>499</v>
+        <v>407</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>499</v>
+        <v>407</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>500</v>
+        <v>408</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>501</v>
+        <v>409</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>502</v>
+        <v>410</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>503</v>
+        <v>411</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>504</v>
+        <v>412</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>505</v>
+        <v>413</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>506</v>
+        <v>414</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>507</v>
+        <v>415</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>508</v>
+        <v>416</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>417</v>
       </c>
       <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>510</v>
+        <v>418</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>509</v>
+        <v>417</v>
       </c>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>511</v>
+        <v>419</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>512</v>
+        <v>420</v>
       </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>513</v>
+        <v>421</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
-        <v>509</v>
+        <v>393</v>
       </c>
       <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>514</v>
+        <v>422</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>509</v>
+        <v>423</v>
       </c>
       <c r="D65" s="1"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>515</v>
+        <v>424</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>488</v>
+        <v>423</v>
       </c>
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>516</v>
+        <v>425</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>517</v>
+        <v>397</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>518</v>
+        <v>393</v>
       </c>
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>519</v>
+        <v>426</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>518</v>
+        <v>393</v>
       </c>
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>520</v>
+        <v>427</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>489</v>
+        <v>428</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>521</v>
+        <v>429</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>522</v>
+        <v>430</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>523</v>
+        <v>431</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>524</v>
+        <v>432</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>525</v>
+        <v>433</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D76" s="1"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>526</v>
+        <v>434</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>485</v>
+        <v>396</v>
       </c>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>527</v>
+        <v>435</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>485</v>
+        <v>396</v>
       </c>
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>528</v>
+        <v>436</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>485</v>
+        <v>396</v>
       </c>
       <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>529</v>
+        <v>437</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D80" s="1"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>530</v>
+        <v>438</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
-        <v>488</v>
+        <v>439</v>
       </c>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>531</v>
+        <v>440</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
-        <v>488</v>
+        <v>393</v>
       </c>
       <c r="D82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>532</v>
+        <v>441</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D83" s="1"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>533</v>
+        <v>442</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>534</v>
+        <v>396</v>
       </c>
       <c r="D84" s="1"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>535</v>
+        <v>443</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>536</v>
+        <v>396</v>
       </c>
       <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>537</v>
+        <v>444</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D86" s="1"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>538</v>
+        <v>445</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D87" s="1"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>539</v>
+        <v>446</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="D88" s="1"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>540</v>
+        <v>447</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
-        <v>488</v>
+        <v>393</v>
       </c>
       <c r="D89" s="1"/>
     </row>
     <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>541</v>
+        <v>445</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="D90" s="1"/>
-    </row>
-    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="D91" s="1"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="D92" s="1"/>
-    </row>
-    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="D93" s="1"/>
-    </row>
-    <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="D94" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>